<commit_message>
Practica 2023 info2 gr2
</commit_message>
<xml_diff>
--- a/ama1-2020.xlsx
+++ b/ama1-2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axa\Documents\Reps\andrei-rusu-ovidius.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC3ED4C-AC46-48F7-BA47-FD7A02F02221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B464E082-515E-4520-A249-0AA9CCDE69CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24A2DEF5-1163-4D13-9934-BD9B9156C910}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{24A2DEF5-1163-4D13-9934-BD9B9156C910}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -362,7 +362,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -467,7 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -481,7 +481,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{9E2DD13D-DD83-4B21-9A10-7EDCDF8DEF5D}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -792,19 +794,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD174EF-646E-49DC-BAEA-894662167010}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="4"/>
-    <col min="2" max="2" width="31.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.7265625" style="2"/>
-    <col min="5" max="5" width="42.36328125" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="4"/>
+    <col min="2" max="2" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.77734375" style="2"/>
+    <col min="5" max="5" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>105</v>
       </c>
@@ -813,7 +815,7 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>107</v>
       </c>
@@ -822,7 +824,7 @@
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>106</v>
       </c>
@@ -831,7 +833,7 @@
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -851,7 +853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -871,7 +873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -891,7 +893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>3</v>
       </c>
@@ -911,7 +913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>4</v>
       </c>
@@ -931,7 +933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>5</v>
       </c>
@@ -951,7 +953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>6</v>
       </c>
@@ -971,7 +973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>7</v>
       </c>
@@ -991,7 +993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>8</v>
       </c>
@@ -1011,7 +1013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>9</v>
       </c>
@@ -1031,7 +1033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>10</v>
       </c>
@@ -1051,7 +1053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>11</v>
       </c>
@@ -1071,7 +1073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>12</v>
       </c>
@@ -1091,7 +1093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>13</v>
       </c>
@@ -1111,7 +1113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>14</v>
       </c>
@@ -1131,7 +1133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>15</v>
       </c>
@@ -1151,7 +1153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>16</v>
       </c>
@@ -1171,7 +1173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>17</v>
       </c>
@@ -1191,7 +1193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>18</v>
       </c>
@@ -1211,7 +1213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>19</v>
       </c>
@@ -1231,7 +1233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>20</v>
       </c>
@@ -1251,7 +1253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>21</v>
       </c>
@@ -1271,7 +1273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>22</v>
       </c>
@@ -1291,7 +1293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>23</v>
       </c>
@@ -1311,7 +1313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>24</v>
       </c>
@@ -1331,7 +1333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>25</v>
       </c>
@@ -1351,7 +1353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>26</v>
       </c>
@@ -1371,7 +1373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>27</v>
       </c>
@@ -1391,7 +1393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>28</v>
       </c>
@@ -1411,7 +1413,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>29</v>
       </c>
@@ -1431,7 +1433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>30</v>
       </c>
@@ -1451,7 +1453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>31</v>
       </c>
@@ -1471,7 +1473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>32</v>
       </c>
@@ -1491,7 +1493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>33</v>
       </c>
@@ -1511,7 +1513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>34</v>
       </c>
@@ -1531,7 +1533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>35</v>
       </c>
@@ -1551,7 +1553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>36</v>
       </c>
@@ -1571,7 +1573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>37</v>
       </c>
@@ -1591,7 +1593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>38</v>
       </c>
@@ -1611,7 +1613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>39</v>
       </c>
@@ -1631,7 +1633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>40</v>
       </c>
@@ -1651,7 +1653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>41</v>
       </c>
@@ -1671,7 +1673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>42</v>
       </c>
@@ -1691,7 +1693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>43</v>
       </c>
@@ -1711,7 +1713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>44</v>
       </c>
@@ -1731,7 +1733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>45</v>
       </c>
@@ -1751,7 +1753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="1" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>46</v>
       </c>
@@ -1771,7 +1773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>47</v>
       </c>
@@ -1791,7 +1793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>48</v>
       </c>
@@ -1809,7 +1811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>49</v>
       </c>
@@ -1827,7 +1829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>50</v>
       </c>
@@ -1845,7 +1847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>55</v>
       </c>
@@ -1857,6 +1859,6 @@
     <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>